<commit_message>
add leetcode array 2 problems
</commit_message>
<xml_diff>
--- a/OJ/LeetCode/status.xlsx
+++ b/OJ/LeetCode/status.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Status</t>
   </si>
@@ -62,7 +62,7 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>?</t>
+    <t>??y</t>
   </si>
   <si>
     <t>1480. Running Sum of 1d Array</t>
@@ -71,16 +71,40 @@
     <t>Array</t>
   </si>
   <si>
-    <t>from end to start</t>
-  </si>
-  <si>
-    <t>+</t>
+    <t>from end to start, 注意i的自增，总是忘掉</t>
+  </si>
+  <si>
+    <t>+y</t>
   </si>
   <si>
     <t>1470. Shuffle the Array</t>
   </si>
   <si>
     <t>vector.push_back()</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>1351. Count Negative Numbers in a Sorted Matrix</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>没有使用二分法，明早起来使用二分法做一下</t>
+  </si>
+  <si>
+    <t>1313. Decompress Run-Length Encoded List</t>
+  </si>
+  <si>
+    <t>？</t>
+  </si>
+  <si>
+    <t>1389. Create Target Array in the Given Order</t>
+  </si>
+  <si>
+    <t>细心，容易将数组中的值弄混, 注意vector.insert(it, value)用法</t>
   </si>
 </sst>
 </file>
@@ -89,9 +113,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -110,6 +134,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -117,15 +148,68 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -141,30 +225,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -179,60 +256,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -272,19 +296,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,157 +470,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,41 +484,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -540,15 +534,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -557,158 +542,200 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1030,20 +1057,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="3"/>
   <cols>
-    <col min="2" max="2" width="30.125" customWidth="1"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="47.875" customWidth="1"/>
+    <col min="3" max="3" width="14.25" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1057,7 +1086,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -1071,7 +1100,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
@@ -1082,6 +1111,48 @@
       </c>
       <c r="D3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>